<commit_message>
a few minor fixes
</commit_message>
<xml_diff>
--- a/data/totem_animals_db.xlsx
+++ b/data/totem_animals_db.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\user\PycharmProjects\Skillfactory\totem_zooanimal_bot\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\user\PycharmProjects\Skillfactory\totem_zooanimal_bot\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13931A7B-B38F-4107-8868-096FE5D02610}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{497BF110-5AB4-4E87-814E-B54E4E7D51F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{410180BA-4176-42AC-8B98-59B9183C5536}"/>
   </bookViews>
@@ -296,7 +296,7 @@
     <t>Удивительные жители тропических лесов Африки, восхитительны не только своей красотой, но и социальной организованностью. Предпочитают жить в крупных группах, где царит строгая иерархия. Мандрилы обладают превосходным чутьем и интеллектом, что позволяет им уверенно навигироваться в густой листве и находить пищу. Их ярко окрашенные морды и впечатляющие клыки делают этих приматов поистине уникальными существами с завораживающим характером.</t>
   </si>
   <si>
-    <t>Настоящий мастер маскировки и остроумный обитатель  Северной Америки. Обычно живущет один, предпочитает оставаться в тени и избегать встреч с другими животными. Блестяще приспособлен к защите себя от хищников благодаря выбиванию неприятных запахов из специальных желез. Своим скрытным образом жизни и уникальными защитными механизмами полосатый скунс создает живописный образ загадочного хищника.</t>
+    <t>Настоящий мастер маскировки и остроумный обитатель  Северной Америки. Обычно живет один, предпочитает оставаться в тени и избегать встреч с другими животными. Блестяще приспособлен к защите себя от хищников благодаря выбиванию неприятных запахов из специальных желез. Своим скрытным образом жизни и уникальными защитными механизмами полосатый скунс создает живописный образ загадочного хищника.</t>
   </si>
 </sst>
 </file>
@@ -689,7 +689,7 @@
   <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>